<commit_message>
Fixed some two inverter issues
</commit_message>
<xml_diff>
--- a/Sungrow_combinations.xlsx
+++ b/Sungrow_combinations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\mkaiser\Sungrow-SHx-Inverter-Modbus-Home-Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F2AB2-4454-4F8D-AD01-2F7248B5177E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404F591B-7AF4-4555-AC86-5112D5D71784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{C6DDEDB4-D689-43D9-B4AA-C92AED3F6D7C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="243">
   <si>
     <t>Battery</t>
   </si>
@@ -407,15 +407,6 @@
   </si>
   <si>
     <t>SG Total DC power</t>
-  </si>
-  <si>
-    <t>SG Load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG1 Total Load Energy </t>
-  </si>
-  <si>
-    <t>SG Total Load Energy</t>
   </si>
   <si>
     <t>SG1 Daily PV generation &amp; battery discharge</t>
@@ -733,20 +724,92 @@
     <t>SG1 Set min SoC reg</t>
   </si>
   <si>
-    <t>hier weiter</t>
-  </si>
-  <si>
     <t>SG Daily PV generation</t>
   </si>
   <si>
     <t>SG Total PV generation</t>
+  </si>
+  <si>
+    <t>basic_sensors.yaml</t>
+  </si>
+  <si>
+    <t>basic_sensors_sg.yaml</t>
+  </si>
+  <si>
+    <t>basic_sensors_sh.yaml</t>
+  </si>
+  <si>
+    <t>basic_automation.yaml</t>
+  </si>
+  <si>
+    <t>basic_input_number.yaml</t>
+  </si>
+  <si>
+    <t>basic_input_select.yaml</t>
+  </si>
+  <si>
+    <t>basic_template_binary_sensor_sg.yaml</t>
+  </si>
+  <si>
+    <t>basic_template_binary_sensor_sh.yaml</t>
+  </si>
+  <si>
+    <t>basic_template_sensor_sg.yaml</t>
+  </si>
+  <si>
+    <t>basic_template_sensor_sh.yaml</t>
+  </si>
+  <si>
+    <t>basic_template_sensor.yaml</t>
+  </si>
+  <si>
+    <t>extended_sensors.yaml</t>
+  </si>
+  <si>
+    <t>extended_template_sensor.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_automation.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_input_number.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_input_select.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_sensors.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_template_binary_sensor.yaml</t>
+  </si>
+  <si>
+    <t>generic_battery_template_sensor.yaml</t>
+  </si>
+  <si>
+    <t>second_inverter_basic_sensor.yaml</t>
+  </si>
+  <si>
+    <t>second_inverter_basic_template_binary_sensor.yaml</t>
+  </si>
+  <si>
+    <t>second_inverter_basic_template_sensor.yaml</t>
+  </si>
+  <si>
+    <t>SG1 Total dissipated energy</t>
+  </si>
+  <si>
+    <t>SG Total Dissipated Energy</t>
+  </si>
+  <si>
+    <t>SG Load power</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -810,8 +873,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -883,7 +954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -911,6 +982,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -926,7 +1000,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1276,7 +1357,7 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
@@ -1296,7 +1377,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -1314,10 +1395,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="9" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1416,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="9" t="s">
         <v>58</v>
       </c>
@@ -1353,7 +1434,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>47</v>
       </c>
@@ -1374,10 +1455,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="9" t="s">
         <v>45</v>
       </c>
@@ -1395,7 +1476,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="9" t="s">
         <v>59</v>
       </c>
@@ -1413,7 +1494,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="14"/>
       <c r="B12" t="s">
         <v>48</v>
       </c>
@@ -1434,10 +1515,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" t="s">
         <v>46</v>
       </c>
@@ -1458,7 +1539,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" t="s">
         <v>60</v>
       </c>
@@ -1479,7 +1560,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>50</v>
       </c>
@@ -1500,15 +1581,15 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
+      <c r="B21" s="15"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
@@ -1530,798 +1611,925 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328AAD0E-C03F-4E5E-8B52-68C7A7F3572A}">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44" customWidth="1"/>
-    <col min="6" max="6" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32" customWidth="1"/>
-    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="17" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="21"/>
+      <c r="E4" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="K5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F6" t="s">
-        <v>163</v>
-      </c>
-      <c r="H6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>164</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="K8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="D8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="D9" t="s">
+      <c r="C9" s="12"/>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" t="s">
+        <v>162</v>
+      </c>
+      <c r="K9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="G10" t="s">
         <v>68</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" t="s">
+        <v>166</v>
+      </c>
+      <c r="K12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" t="s">
         <v>131</v>
       </c>
-      <c r="F9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="I13" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" t="s">
         <v>132</v>
       </c>
-      <c r="F10" t="s">
-        <v>167</v>
-      </c>
-      <c r="H10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" t="s">
+      <c r="I14" t="s">
+        <v>168</v>
+      </c>
+      <c r="K14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" t="s">
         <v>133</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I15" t="s">
         <v>169</v>
       </c>
-      <c r="H11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" t="s">
+      <c r="K15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
         <v>134</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I16" t="s">
         <v>170</v>
       </c>
-      <c r="H12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" t="s">
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
         <v>135</v>
       </c>
-      <c r="F13" t="s">
+      <c r="I17" t="s">
         <v>171</v>
       </c>
-      <c r="H13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" t="s">
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" t="s">
         <v>136</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I18" t="s">
         <v>172</v>
       </c>
-      <c r="H14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
         <v>137</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" t="s">
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s">
         <v>138</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I20" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s">
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" t="s">
         <v>139</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I21" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
         <v>140</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I22" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" t="s">
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" t="s">
         <v>141</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" t="s">
         <v>142</v>
       </c>
-      <c r="F20" t="s">
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>84</v>
+      </c>
+      <c r="I28" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" t="s">
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D41" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D42" s="13"/>
+      <c r="E42" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" t="s">
+        <v>86</v>
+      </c>
+      <c r="I43" t="s">
+        <v>190</v>
+      </c>
+      <c r="K43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" t="s">
+        <v>87</v>
+      </c>
+      <c r="I44" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D47" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D48" s="13"/>
+      <c r="E48" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>89</v>
+      </c>
+      <c r="H49" t="s">
         <v>143</v>
       </c>
-      <c r="F21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="I49" t="s">
+        <v>192</v>
+      </c>
+      <c r="K49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" t="s">
         <v>144</v>
       </c>
-      <c r="F22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="I50" t="s">
+        <v>193</v>
+      </c>
+      <c r="K50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>91</v>
+      </c>
+      <c r="H51" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F38" t="s">
+      <c r="I51" t="s">
+        <v>194</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" t="s">
+        <v>146</v>
+      </c>
+      <c r="I52" t="s">
+        <v>195</v>
+      </c>
+      <c r="K52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>93</v>
+      </c>
+      <c r="H53" t="s">
+        <v>147</v>
+      </c>
+      <c r="I53" t="s">
+        <v>196</v>
+      </c>
+      <c r="K53" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>94</v>
+      </c>
+      <c r="H54" t="s">
+        <v>148</v>
+      </c>
+      <c r="I54" t="s">
+        <v>197</v>
+      </c>
+      <c r="K54" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>95</v>
+      </c>
+      <c r="H55" t="s">
+        <v>149</v>
+      </c>
+      <c r="I55" t="s">
+        <v>198</v>
+      </c>
+      <c r="K55" s="22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>96</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>150</v>
+      </c>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G58" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H58" t="s">
+        <v>151</v>
+      </c>
+      <c r="I58" s="10"/>
+      <c r="K58" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G59" s="8"/>
+      <c r="H59" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G60" s="8"/>
+      <c r="H60" t="s">
+        <v>153</v>
+      </c>
+      <c r="K60" s="10"/>
+    </row>
+    <row r="61" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D62" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+    </row>
+    <row r="63" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+    </row>
+    <row r="64" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>98</v>
+      </c>
+      <c r="I64" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I67" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D74" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
+    </row>
+    <row r="75" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
+    </row>
+    <row r="76" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>55</v>
+      </c>
+      <c r="I76" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" t="s">
-        <v>193</v>
-      </c>
-      <c r="H41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" t="s">
-        <v>146</v>
-      </c>
-      <c r="F46" t="s">
-        <v>195</v>
-      </c>
-      <c r="H46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" t="s">
-        <v>196</v>
-      </c>
-      <c r="H47" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" t="s">
-        <v>148</v>
-      </c>
-      <c r="F48" t="s">
-        <v>197</v>
-      </c>
-      <c r="H48" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>92</v>
-      </c>
-      <c r="E49" t="s">
-        <v>149</v>
-      </c>
-      <c r="F49" t="s">
-        <v>198</v>
-      </c>
-      <c r="H49" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
+      <c r="K76" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
         <v>93</v>
       </c>
-      <c r="E50" t="s">
-        <v>150</v>
-      </c>
-      <c r="F50" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E51" t="s">
-        <v>151</v>
-      </c>
-      <c r="F51" t="s">
-        <v>200</v>
-      </c>
-      <c r="H51" s="18" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52" t="s">
-        <v>152</v>
-      </c>
-      <c r="F52" t="s">
-        <v>201</v>
-      </c>
-      <c r="H52" s="18" t="s">
+    </row>
+    <row r="80" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D80" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+      <c r="L80" s="16"/>
+    </row>
+    <row r="81" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>96</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>153</v>
-      </c>
-      <c r="F54" s="10"/>
-      <c r="H54" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E55" t="s">
-        <v>154</v>
-      </c>
-      <c r="F55" s="10"/>
-      <c r="H55" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D56" s="8"/>
-      <c r="E56" t="s">
-        <v>155</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="8"/>
-      <c r="E57" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F61" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F62" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F63" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F64" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F65" t="s">
+      <c r="H81" s="13"/>
+      <c r="I81" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+    </row>
+    <row r="82" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>99</v>
+      </c>
+      <c r="I82" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F66" t="s">
+      <c r="K82" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>100</v>
+      </c>
+      <c r="I83" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>101</v>
+      </c>
+      <c r="I84" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F67" t="s">
+    <row r="85" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>121</v>
+      </c>
+      <c r="I85" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>55</v>
-      </c>
-      <c r="F71" t="s">
-        <v>195</v>
-      </c>
-      <c r="H71" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D76" t="s">
-        <v>99</v>
-      </c>
-      <c r="F76" t="s">
+    <row r="86" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
         <v>210</v>
       </c>
-      <c r="H76" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>100</v>
-      </c>
-      <c r="F77" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>101</v>
-      </c>
-      <c r="F78" t="s">
+    </row>
+    <row r="87" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>121</v>
-      </c>
-      <c r="F79" t="s">
+    <row r="88" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F80" t="s">
+    <row r="89" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F81" t="s">
+    <row r="90" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F82" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F83" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F84" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B59:I59"/>
-    <mergeCell ref="B70:I70"/>
-    <mergeCell ref="B75:I75"/>
-    <mergeCell ref="B26:I26"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B45:I45"/>
+    <mergeCell ref="D62:L62"/>
+    <mergeCell ref="D74:L74"/>
+    <mergeCell ref="D80:L80"/>
+    <mergeCell ref="D27:L27"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D41:L41"/>
+    <mergeCell ref="D47:L47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>